<commit_message>
adding log4j and testng xml file
</commit_message>
<xml_diff>
--- a/src/test/resources/ClientTestData.xlsx
+++ b/src/test/resources/ClientTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hendy\Desktop\FW_Skeleton\RestAssuredT\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BCBB07-2D39-4779-A69A-FE2FC76B9737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300CE439-5819-4BB1-8A34-A5BE12FB29B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,16 +33,16 @@
     <t>clientEmail</t>
   </si>
   <si>
-    <t>moh6</t>
-  </si>
-  <si>
-    <t>moh6@h.com</t>
-  </si>
-  <si>
-    <t>moh7</t>
-  </si>
-  <si>
-    <t>moh7@h.com</t>
+    <t>moh6q</t>
+  </si>
+  <si>
+    <t>moh7q</t>
+  </si>
+  <si>
+    <t>moh79@qh.com</t>
+  </si>
+  <si>
+    <t>hen97@qh.com</t>
   </si>
 </sst>
 </file>
@@ -374,7 +374,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,12 +396,12 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
adding listeners plus adding maven plugins plus adding allure report features
</commit_message>
<xml_diff>
--- a/src/test/resources/ClientTestData.xlsx
+++ b/src/test/resources/ClientTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hendy\Desktop\FW_Skeleton\RestAssuredT\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300CE439-5819-4BB1-8A34-A5BE12FB29B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CECA2C-6222-4F27-9899-4EFF4844E845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>clientName</t>
   </si>
@@ -36,13 +36,7 @@
     <t>moh6q</t>
   </si>
   <si>
-    <t>moh7q</t>
-  </si>
-  <si>
-    <t>moh79@qh.com</t>
-  </si>
-  <si>
-    <t>hen97@qh.com</t>
+    <t>hendi59@qh.com</t>
   </si>
 </sst>
 </file>
@@ -371,10 +365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,21 +390,12 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{F2F8CB37-3D5E-4153-973E-17B9C6585405}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{84AD4D62-A8A2-4F06-A267-7EBF18719665}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding new test data
</commit_message>
<xml_diff>
--- a/src/test/resources/ClientTestData.xlsx
+++ b/src/test/resources/ClientTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hendy\Desktop\FW_Skeleton\RestAssuredT\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CECA2C-6222-4F27-9899-4EFF4844E845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C071FE81-E111-4E2F-B778-924E2C68FFD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,17 +34,17 @@
     <t>clientEmail</t>
   </si>
   <si>
-    <t>moh6q</t>
+    <t>hendi39@qh.com4</t>
   </si>
   <si>
-    <t>hendi59@qh.com</t>
+    <t>jenkins</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,6 +56,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -368,7 +375,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -387,13 +394,14 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{F2F8CB37-3D5E-4153-973E-17B9C6585405}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
adding new test data for jenkins 1
</commit_message>
<xml_diff>
--- a/src/test/resources/ClientTestData.xlsx
+++ b/src/test/resources/ClientTestData.xlsx
@@ -8,18 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hendy\Desktop\FW_Skeleton\RestAssuredT\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C071FE81-E111-4E2F-B778-924E2C68FFD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681521B1-CDBD-4F8D-93FB-FF8B4C0E2F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -34,10 +45,10 @@
     <t>clientEmail</t>
   </si>
   <si>
-    <t>hendi39@qh.com4</t>
+    <t>jenkins</t>
   </si>
   <si>
-    <t>jenkins</t>
+    <t>hendi19@qh.com4</t>
   </si>
 </sst>
 </file>
@@ -375,7 +386,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,10 +405,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding new test data312
</commit_message>
<xml_diff>
--- a/src/test/resources/ClientTestData.xlsx
+++ b/src/test/resources/ClientTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hendy\Desktop\FW_Skeleton\RestAssuredT\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681521B1-CDBD-4F8D-93FB-FF8B4C0E2F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7A9944-8AFE-4C1F-AA05-B4C239DB9894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,7 +47,7 @@
     <t>jenkins</t>
   </si>
   <si>
-    <t>hendi19@qh.com4</t>
+    <t>hendi18@qh.com4</t>
   </si>
 </sst>
 </file>
@@ -386,7 +385,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>